<commit_message>
17 Babel. Extract plugin [optional] для переводов i18n
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E3563-1F2D-4A03-B6F3-832D8C3EC4BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFF1C7B-6452-4210-9AE8-0CCECC2E38E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,8 +651,8 @@
   <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +664,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="2">
         <f>SUM(B2:B177)</f>
-        <v>2.2225925925925929</v>
+        <v>1.0876620370370367</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1027,7 +1027,7 @@
         <v>41</v>
       </c>
       <c r="B53" s="2">
-        <v>1.1541666666666666</v>
+        <v>1.923611111111111E-2</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
46 React refresh plugin
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874C69E0-7B73-4E60-BF11-3477C152D1E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB4849C-167F-4E07-9063-A972D85A2AE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,8 +651,8 @@
   <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1048,7 @@
       <c r="A57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="4">
         <v>5.1388888888888894E-2</v>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       <c r="A58" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="4">
         <v>7.6736111111111111E-3</v>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       <c r="A59" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="4">
         <v>2.2511574074074073E-2</v>
       </c>
     </row>
@@ -1072,7 +1072,7 @@
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="4">
         <v>3.2407407407407406E-3</v>
       </c>
     </row>
@@ -1080,7 +1080,7 @@
       <c r="A61" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="4">
         <v>4.5138888888888893E-3</v>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       <c r="A62" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="4">
         <v>4.3981481481481484E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
91 Testing public api. Micromatch. Тесты на eslint плагин
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F508FFF4-FA21-4F8D-AE65-78ECD756BABC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834022F6-4063-433F-96DD-2332AB6099DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,8 +886,8 @@
   <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B117" sqref="B117:B190"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1694,7 +1694,7 @@
       <c r="A117" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="4">
         <v>5.208333333333333E-3</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       <c r="A118" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118" s="4">
         <v>5.9606481481481489E-3</v>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
       <c r="A119" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="4">
         <v>8.7962962962962968E-3</v>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
       <c r="A120" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="4">
         <v>7.8356481481481489E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
105 BuildSlice. BuildSelector. Улучшаем работу со state. useActions
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834022F6-4063-433F-96DD-2332AB6099DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF647CD-6EBE-4A7C-B879-4FFED35FA667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,8 +886,8 @@
   <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134:B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,7 +1726,7 @@
       <c r="A121" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="4">
         <v>2.5462962962962961E-3</v>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
       <c r="A122" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="4">
         <v>1.2268518518518519E-2</v>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       <c r="A123" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123" s="4">
         <v>8.7615740740740744E-3</v>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       <c r="A124" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124" s="4">
         <v>1.5856481481481479E-3</v>
       </c>
     </row>
@@ -1758,7 +1758,7 @@
       <c r="A125" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125" s="4">
         <v>5.0810185185185186E-3</v>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       <c r="A126" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126" s="4">
         <v>6.8171296296296287E-3</v>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
       <c r="A127" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127" s="4">
         <v>4.0277777777777777E-3</v>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
       <c r="A128" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128" s="4">
         <v>2.6620370370370374E-3</v>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       <c r="A129" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129" s="4">
         <v>2.3379629629629631E-3</v>
       </c>
     </row>
@@ -1798,7 +1798,7 @@
       <c r="A130" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="4">
         <v>1.8402777777777777E-3</v>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       <c r="A131" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131" s="4">
         <v>4.8611111111111112E-3</v>
       </c>
     </row>
@@ -1814,7 +1814,7 @@
       <c r="A132" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132" s="4">
         <v>3.9351851851851857E-3</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       <c r="A133" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133" s="4">
         <v>6.053240740740741E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
137 addon left right. Инпут, кнопка. Pixel perfect plugin проверка
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C58DA71-D931-4E75-8FC7-8A7E3CB5230A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C75DB4-1E77-40D6-961E-801414B1AE41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,8 +886,8 @@
   <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B157" sqref="B157:B164"/>
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B173" sqref="B173:B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2061,7 +2061,7 @@
       <c r="A167" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B167" s="4">
         <v>2.2372685185185186E-2</v>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       <c r="A168" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B168" s="4">
         <v>4.2939814814814811E-3</v>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       <c r="A169" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B169" s="4">
         <v>3.6805555555555554E-3</v>
       </c>
     </row>
@@ -2085,7 +2085,7 @@
       <c r="A170" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B170" s="4">
         <v>2.3391203703703702E-2</v>
       </c>
     </row>
@@ -2093,7 +2093,7 @@
       <c r="A171" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B171" s="4">
         <v>1.6701388888888887E-2</v>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       <c r="A172" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B172" s="4">
         <v>2.5543981481481483E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
151 Toolbar как часть Layout. ScrollToolbar. useCurrentRoute
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03459C1-FAA8-4CBA-9E75-A335F9C57408}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51379CE0-9A66-429F-B111-B388C2FBE1F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="173">
   <si>
     <t>2 Декомпозиция конфига. Опции конфигурации</t>
   </si>
@@ -887,7 +887,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B180" sqref="B180:B183"/>
+      <selection pane="bottomLeft" activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2197,7 +2197,7 @@
       <c r="A184" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="4">
         <v>6.5509259259259262E-3</v>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
       <c r="A185" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="4">
         <v>3.472222222222222E-3</v>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       <c r="A186" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186" s="4">
         <v>6.3888888888888884E-3</v>
       </c>
     </row>
@@ -2221,7 +2221,7 @@
       <c r="A187" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B187" s="4">
         <v>8.4259259259259253E-3</v>
       </c>
     </row>

</xml_diff>